<commit_message>
Changes to forecast and running the FIM (03/24)
</commit_message>
<xml_diff>
--- a/results/03-2024/comparison-deflators-03-2024.xlsx
+++ b/results/03-2024/comparison-deflators-03-2024.xlsx
@@ -608,16 +608,16 @@
         <v>0.0064</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0045</v>
+        <v>0.0044</v>
       </c>
       <c r="N2" t="n">
-        <v>0.0046</v>
+        <v>0.0074</v>
       </c>
       <c r="O2" t="n">
-        <v>0.0053</v>
+        <v>0.0067</v>
       </c>
       <c r="P2" t="n">
-        <v>0.0055</v>
+        <v>0.006</v>
       </c>
       <c r="Q2" t="n">
         <v>0.0055</v>
@@ -759,7 +759,7 @@
         <v>-0.029</v>
       </c>
       <c r="R4" t="n">
-        <v>-0.0281</v>
+        <v>-0.028</v>
       </c>
       <c r="S4" t="n">
         <v>-0.0264</v>
@@ -812,34 +812,34 @@
         <v>-0.0421</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.2947</v>
+        <v>0.1538</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.2553</v>
+        <v>-0.2559</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.4625</v>
+        <v>-0.4623</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.0666</v>
+        <v>-0.0669</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.083</v>
+        <v>-0.0832</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.4212</v>
+        <v>-0.4215</v>
       </c>
       <c r="S5" t="n">
-        <v>-0.2973</v>
+        <v>-0.2976</v>
       </c>
       <c r="T5" t="n">
-        <v>-0.1303</v>
+        <v>-0.1307</v>
       </c>
       <c r="U5" t="n">
-        <v>-0.166</v>
+        <v>-0.1664</v>
       </c>
       <c r="V5" t="n">
-        <v>-1.9434</v>
+        <v>-1.9431</v>
       </c>
     </row>
     <row r="6">
@@ -880,34 +880,34 @@
         <v>0.3088</v>
       </c>
       <c r="M6" t="n">
-        <v>0.2804</v>
+        <v>0.2796</v>
       </c>
       <c r="N6" t="n">
-        <v>0.1638</v>
+        <v>0.16</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.1183</v>
+        <v>-0.1199</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.2381</v>
+        <v>-0.2378</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.2242</v>
+        <v>-0.2232</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.2846</v>
+        <v>-0.2835</v>
       </c>
       <c r="S6" t="n">
-        <v>-0.2202</v>
+        <v>-0.2191</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.1713</v>
+        <v>-0.1703</v>
       </c>
       <c r="U6" t="n">
-        <v>-0.0359</v>
+        <v>-0.035</v>
       </c>
       <c r="V6" t="n">
-        <v>-0.7425</v>
+        <v>-0.7412</v>
       </c>
     </row>
     <row r="7">
@@ -948,34 +948,34 @@
         <v>-0.2751</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.1625</v>
+        <v>-0.1622</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.2623</v>
+        <v>-0.2326</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.2571</v>
+        <v>-0.2193</v>
       </c>
       <c r="P7" t="n">
-        <v>-0.0697</v>
+        <v>-0.0199</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.1072</v>
+        <v>-0.0569</v>
       </c>
       <c r="R7" t="n">
-        <v>-0.0109</v>
+        <v>0.0123</v>
       </c>
       <c r="S7" t="n">
-        <v>0.0136</v>
+        <v>0.0299</v>
       </c>
       <c r="T7" t="n">
-        <v>0.0369</v>
+        <v>0.0425</v>
       </c>
       <c r="U7" t="n">
-        <v>0.0515</v>
+        <v>0.056</v>
       </c>
       <c r="V7" t="n">
-        <v>0.0668</v>
+        <v>0.0702</v>
       </c>
     </row>
     <row r="8">
@@ -1016,34 +1016,34 @@
         <v>0.3669</v>
       </c>
       <c r="M8" t="n">
-        <v>0.3655</v>
+        <v>0.3659</v>
       </c>
       <c r="N8" t="n">
-        <v>0.2297</v>
+        <v>0.2453</v>
       </c>
       <c r="O8" t="n">
-        <v>0.1811</v>
+        <v>0.2073</v>
       </c>
       <c r="P8" t="n">
-        <v>0.3253</v>
+        <v>0.3473</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.2391</v>
+        <v>0.2554</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.1013</v>
+        <v>-0.0867</v>
       </c>
       <c r="S8" t="n">
-        <v>-0.1198</v>
+        <v>-0.1053</v>
       </c>
       <c r="T8" t="n">
-        <v>-0.0931</v>
+        <v>-0.079</v>
       </c>
       <c r="U8" t="n">
-        <v>-0.0867</v>
+        <v>-0.073</v>
       </c>
       <c r="V8" t="n">
-        <v>-0.0102</v>
+        <v>-0.0034</v>
       </c>
     </row>
     <row r="9">
@@ -1161,13 +1161,13 @@
         <v>-0.0488</v>
       </c>
       <c r="P10" t="n">
-        <v>-0.0432</v>
+        <v>-0.0433</v>
       </c>
       <c r="Q10" t="n">
         <v>-0.0257</v>
       </c>
       <c r="R10" t="n">
-        <v>-0.0102</v>
+        <v>-0.0103</v>
       </c>
       <c r="S10" t="n">
         <v>-0.0098</v>
@@ -1220,7 +1220,7 @@
         <v>0.0098</v>
       </c>
       <c r="M11" t="n">
-        <v>0.01</v>
+        <v>0.0098</v>
       </c>
       <c r="N11" t="n">
         <v>0.0059</v>
@@ -1288,34 +1288,34 @@
         <v>0.0114</v>
       </c>
       <c r="M12" t="n">
-        <v>-0.1543</v>
+        <v>-0.1481</v>
       </c>
       <c r="N12" t="n">
-        <v>-0.1614</v>
+        <v>-0.173</v>
       </c>
       <c r="O12" t="n">
-        <v>-0.0594</v>
+        <v>-0.0803</v>
       </c>
       <c r="P12" t="n">
-        <v>-0.0121</v>
+        <v>-0.036</v>
       </c>
       <c r="Q12" t="n">
-        <v>-0.0002</v>
+        <v>-0.0298</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.044</v>
+        <v>-0.0563</v>
       </c>
       <c r="S12" t="n">
-        <v>-0.0481</v>
+        <v>-0.0513</v>
       </c>
       <c r="T12" t="n">
-        <v>-0.0504</v>
+        <v>-0.0506</v>
       </c>
       <c r="U12" t="n">
-        <v>-0.1048</v>
+        <v>-0.105</v>
       </c>
       <c r="V12" t="n">
-        <v>-6.302</v>
+        <v>-6.3047</v>
       </c>
     </row>
     <row r="13">
@@ -1424,34 +1424,34 @@
         <v>-0.3432</v>
       </c>
       <c r="M14" t="n">
-        <v>-0.1407</v>
+        <v>-0.1408</v>
       </c>
       <c r="N14" t="n">
-        <v>-0.1034</v>
+        <v>-0.1035</v>
       </c>
       <c r="O14" t="n">
-        <v>-0.2904</v>
+        <v>-0.2906</v>
       </c>
       <c r="P14" t="n">
-        <v>-0.2614</v>
+        <v>-0.2615</v>
       </c>
       <c r="Q14" t="n">
-        <v>-0.1046</v>
+        <v>-0.1048</v>
       </c>
       <c r="R14" t="n">
-        <v>-0.0568</v>
+        <v>-0.057</v>
       </c>
       <c r="S14" t="n">
-        <v>-0.0915</v>
+        <v>-0.0917</v>
       </c>
       <c r="T14" t="n">
-        <v>-0.0676</v>
+        <v>-0.0677</v>
       </c>
       <c r="U14" t="n">
-        <v>-0.0296</v>
+        <v>-0.0298</v>
       </c>
       <c r="V14" t="n">
-        <v>-0.0777</v>
+        <v>-0.0778</v>
       </c>
     </row>
     <row r="15">
@@ -1560,34 +1560,34 @@
         <v>0.5287</v>
       </c>
       <c r="M16" t="n">
-        <v>0.1869</v>
+        <v>0.2312</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.4043</v>
+        <v>-0.2678</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.7993</v>
+        <v>-0.6669</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.6397</v>
+        <v>-0.4807</v>
       </c>
       <c r="Q16" t="n">
-        <v>-0.3742</v>
+        <v>-0.2571</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.82</v>
+        <v>-0.8043</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.8363</v>
+        <v>-0.8209</v>
       </c>
       <c r="T16" t="n">
-        <v>-0.5322</v>
+        <v>-0.5283</v>
       </c>
       <c r="U16" t="n">
-        <v>-0.3685</v>
+        <v>-0.3389</v>
       </c>
       <c r="V16" t="n">
-        <v>-50.6121</v>
+        <v>-50.7598</v>
       </c>
     </row>
     <row r="17">
@@ -1628,34 +1628,34 @@
         <v>27610.1</v>
       </c>
       <c r="M17" t="n">
-        <v>27944.6</v>
+        <v>27957</v>
       </c>
       <c r="N17" t="n">
-        <v>28264.1826</v>
+        <v>28276.7244</v>
       </c>
       <c r="O17" t="n">
-        <v>28601.9138</v>
+        <v>28614.6055</v>
       </c>
       <c r="P17" t="n">
-        <v>28946.529</v>
+        <v>28959.3736</v>
       </c>
       <c r="Q17" t="n">
-        <v>29303.3476</v>
+        <v>29316.3505</v>
       </c>
       <c r="R17" t="n">
-        <v>29666.9459</v>
+        <v>29680.1101</v>
       </c>
       <c r="S17" t="n">
-        <v>30021.887</v>
+        <v>30035.2088</v>
       </c>
       <c r="T17" t="n">
-        <v>30371.8216</v>
+        <v>30385.2987</v>
       </c>
       <c r="U17" t="n">
-        <v>30709.2399</v>
+        <v>30722.8667</v>
       </c>
       <c r="V17" t="n">
-        <v>31046.8669</v>
+        <v>31060.6435</v>
       </c>
     </row>
     <row r="18">
@@ -1696,34 +1696,34 @@
         <v>-0.3502</v>
       </c>
       <c r="M18" t="n">
-        <v>-0.2978</v>
+        <v>0.1455</v>
       </c>
       <c r="N18" t="n">
-        <v>-0.1183</v>
+        <v>-0.119</v>
       </c>
       <c r="O18" t="n">
-        <v>-0.3518</v>
+        <v>-0.3516</v>
       </c>
       <c r="P18" t="n">
-        <v>-0.0102</v>
+        <v>-0.0106</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.0156</v>
+        <v>0.0153</v>
       </c>
       <c r="R18" t="n">
-        <v>-0.3044</v>
+        <v>-0.3047</v>
       </c>
       <c r="S18" t="n">
-        <v>-0.1891</v>
+        <v>-0.1895</v>
       </c>
       <c r="T18" t="n">
-        <v>-0.0358</v>
+        <v>-0.0363</v>
       </c>
       <c r="U18" t="n">
-        <v>-0.0869</v>
+        <v>-0.0874</v>
       </c>
       <c r="V18" t="n">
-        <v>-1.6968</v>
+        <v>-1.6966</v>
       </c>
     </row>
     <row r="19">
@@ -1841,16 +1841,16 @@
         <v>-0.1051</v>
       </c>
       <c r="P20" t="n">
-        <v>-0.102</v>
+        <v>-0.1019</v>
       </c>
       <c r="Q20" t="n">
-        <v>-0.0999</v>
+        <v>-0.0998</v>
       </c>
       <c r="R20" t="n">
-        <v>-0.0968</v>
+        <v>-0.0967</v>
       </c>
       <c r="S20" t="n">
-        <v>-0.0938</v>
+        <v>-0.0937</v>
       </c>
       <c r="T20" t="n">
         <v>-0.001</v>
@@ -1968,34 +1968,34 @@
         <v>0.6465</v>
       </c>
       <c r="M22" t="n">
-        <v>0.6308</v>
+        <v>0.2484</v>
       </c>
       <c r="N22" t="n">
-        <v>0.0461</v>
+        <v>0.0996</v>
       </c>
       <c r="O22" t="n">
-        <v>0.3614</v>
+        <v>0.3612</v>
       </c>
       <c r="P22" t="n">
-        <v>-0.065</v>
+        <v>-0.0437</v>
       </c>
       <c r="Q22" t="n">
-        <v>-0.0943</v>
+        <v>-0.0625</v>
       </c>
       <c r="R22" t="n">
-        <v>0.2326</v>
+        <v>0.2327</v>
       </c>
       <c r="S22" t="n">
-        <v>0.121</v>
+        <v>0.1212</v>
       </c>
       <c r="T22" t="n">
-        <v>-0.0294</v>
+        <v>-0.0292</v>
       </c>
       <c r="U22" t="n">
-        <v>0.0159</v>
+        <v>0.0161</v>
       </c>
       <c r="V22" t="n">
-        <v>-41.5341</v>
+        <v>-41.6959</v>
       </c>
     </row>
     <row r="23">
@@ -2036,34 +2036,34 @@
         <v>-0.0209</v>
       </c>
       <c r="M23" t="n">
-        <v>-0.018</v>
+        <v>-0.027</v>
       </c>
       <c r="N23" t="n">
-        <v>-0.0163</v>
+        <v>-0.016</v>
       </c>
       <c r="O23" t="n">
-        <v>-0.0125</v>
+        <v>-0.0121</v>
       </c>
       <c r="P23" t="n">
-        <v>-0.005</v>
+        <v>-0.0046</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.0117</v>
+        <v>0.0121</v>
       </c>
       <c r="R23" t="n">
-        <v>0.0258</v>
+        <v>0.0263</v>
       </c>
       <c r="S23" t="n">
-        <v>0.0055</v>
+        <v>0.0059</v>
       </c>
       <c r="T23" t="n">
-        <v>0.0055</v>
+        <v>0.006</v>
       </c>
       <c r="U23" t="n">
-        <v>0.0106</v>
+        <v>0.011</v>
       </c>
       <c r="V23" t="n">
-        <v>0.0154</v>
+        <v>0.0157</v>
       </c>
     </row>
     <row r="24">
@@ -2104,34 +2104,34 @@
         <v>0.219</v>
       </c>
       <c r="M24" t="n">
-        <v>0.017</v>
+        <v>0.0574</v>
       </c>
       <c r="N24" t="n">
-        <v>0.0491</v>
+        <v>0.1506</v>
       </c>
       <c r="O24" t="n">
-        <v>-0.0678</v>
+        <v>0.0366</v>
       </c>
       <c r="P24" t="n">
-        <v>-0.1386</v>
+        <v>-0.0311</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.0267</v>
+        <v>0.0947</v>
       </c>
       <c r="R24" t="n">
-        <v>-0.0564</v>
+        <v>-0.0475</v>
       </c>
       <c r="S24" t="n">
-        <v>-0.0342</v>
+        <v>-0.0287</v>
       </c>
       <c r="T24" t="n">
-        <v>-0.0129</v>
+        <v>-0.0114</v>
       </c>
       <c r="U24" t="n">
-        <v>-0.0064</v>
+        <v>-0.0048</v>
       </c>
       <c r="V24" t="n">
-        <v>0.0002</v>
+        <v>0.0019</v>
       </c>
     </row>
     <row r="25">
@@ -2172,34 +2172,34 @@
         <v>0.1954</v>
       </c>
       <c r="M25" t="n">
-        <v>0.1982</v>
+        <v>0.1388</v>
       </c>
       <c r="N25" t="n">
-        <v>0.2155</v>
+        <v>0.1693</v>
       </c>
       <c r="O25" t="n">
-        <v>0.1739</v>
+        <v>0.163</v>
       </c>
       <c r="P25" t="n">
-        <v>0.1286</v>
+        <v>0.1135</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.0951</v>
+        <v>0.0774</v>
       </c>
       <c r="R25" t="n">
-        <v>0.0543</v>
+        <v>0.0358</v>
       </c>
       <c r="S25" t="n">
-        <v>-0.0199</v>
+        <v>-0.0382</v>
       </c>
       <c r="T25" t="n">
-        <v>0.0079</v>
+        <v>-0.0102</v>
       </c>
       <c r="U25" t="n">
-        <v>-0.0105</v>
+        <v>-0.0014</v>
       </c>
       <c r="V25" t="n">
-        <v>-0.0056</v>
+        <v>-0.0023</v>
       </c>
     </row>
     <row r="26">
@@ -2240,7 +2240,7 @@
         <v>0.0141</v>
       </c>
       <c r="M26" t="n">
-        <v>0.0012</v>
+        <v>0.0016</v>
       </c>
       <c r="N26" t="n">
         <v>0.0074</v>
@@ -2447,25 +2447,25 @@
         <v>-0.0005</v>
       </c>
       <c r="N29" t="n">
-        <v>-0.0011</v>
+        <v>-0.0013</v>
       </c>
       <c r="O29" t="n">
-        <v>0.0046</v>
+        <v>0.0043</v>
       </c>
       <c r="P29" t="n">
-        <v>0.0064</v>
+        <v>0.0061</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.006</v>
+        <v>0.0057</v>
       </c>
       <c r="R29" t="n">
+        <v>0.0059</v>
+      </c>
+      <c r="S29" t="n">
         <v>0.0061</v>
       </c>
-      <c r="S29" t="n">
-        <v>0.0062</v>
-      </c>
       <c r="T29" t="n">
-        <v>0.005</v>
+        <v>0.0049</v>
       </c>
       <c r="U29" t="n">
         <v>0.0024</v>
@@ -2512,16 +2512,16 @@
         <v>0</v>
       </c>
       <c r="M30" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="N30" t="n">
-        <v>0</v>
+        <v>0.0028</v>
       </c>
       <c r="O30" t="n">
-        <v>0</v>
+        <v>0.0015</v>
       </c>
       <c r="P30" t="n">
-        <v>0</v>
+        <v>0.0005</v>
       </c>
       <c r="Q30" t="n">
         <v>0</v>
@@ -2716,34 +2716,34 @@
         <v>0</v>
       </c>
       <c r="M33" t="n">
-        <v>0</v>
+        <v>0.4485</v>
       </c>
       <c r="N33" t="n">
-        <v>0</v>
+        <v>-0.0006</v>
       </c>
       <c r="O33" t="n">
-        <v>0</v>
+        <v>0.0003</v>
       </c>
       <c r="P33" t="n">
-        <v>0</v>
+        <v>-0.0003</v>
       </c>
       <c r="Q33" t="n">
-        <v>0</v>
+        <v>-0.0003</v>
       </c>
       <c r="R33" t="n">
-        <v>0</v>
+        <v>-0.0003</v>
       </c>
       <c r="S33" t="n">
-        <v>0</v>
+        <v>-0.0003</v>
       </c>
       <c r="T33" t="n">
-        <v>0</v>
+        <v>-0.0004</v>
       </c>
       <c r="U33" t="n">
-        <v>0</v>
+        <v>-0.0004</v>
       </c>
       <c r="V33" t="n">
-        <v>0</v>
+        <v>0.0003</v>
       </c>
     </row>
     <row r="34">
@@ -2784,34 +2784,34 @@
         <v>0</v>
       </c>
       <c r="M34" t="n">
-        <v>0</v>
+        <v>-0.0008</v>
       </c>
       <c r="N34" t="n">
-        <v>0</v>
+        <v>-0.0038</v>
       </c>
       <c r="O34" t="n">
-        <v>0</v>
+        <v>-0.0017</v>
       </c>
       <c r="P34" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="Q34" t="n">
-        <v>0</v>
+        <v>0.0011</v>
       </c>
       <c r="R34" t="n">
-        <v>0</v>
+        <v>0.0011</v>
       </c>
       <c r="S34" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="T34" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="U34" t="n">
-        <v>0</v>
+        <v>0.0009</v>
       </c>
       <c r="V34" t="n">
-        <v>0</v>
+        <v>0.0012</v>
       </c>
     </row>
     <row r="35">
@@ -2852,34 +2852,34 @@
         <v>0</v>
       </c>
       <c r="M35" t="n">
-        <v>0</v>
+        <v>0.0003</v>
       </c>
       <c r="N35" t="n">
-        <v>0</v>
+        <v>0.0296</v>
       </c>
       <c r="O35" t="n">
-        <v>0</v>
+        <v>0.0378</v>
       </c>
       <c r="P35" t="n">
-        <v>0</v>
+        <v>0.0497</v>
       </c>
       <c r="Q35" t="n">
-        <v>0</v>
+        <v>0.0503</v>
       </c>
       <c r="R35" t="n">
-        <v>0</v>
+        <v>0.0233</v>
       </c>
       <c r="S35" t="n">
-        <v>0</v>
+        <v>0.0163</v>
       </c>
       <c r="T35" t="n">
-        <v>0</v>
+        <v>0.0056</v>
       </c>
       <c r="U35" t="n">
-        <v>0</v>
+        <v>0.0045</v>
       </c>
       <c r="V35" t="n">
-        <v>0</v>
+        <v>0.0034</v>
       </c>
     </row>
     <row r="36">
@@ -2920,34 +2920,34 @@
         <v>0</v>
       </c>
       <c r="M36" t="n">
-        <v>0</v>
+        <v>0.0004</v>
       </c>
       <c r="N36" t="n">
-        <v>0</v>
+        <v>0.0155</v>
       </c>
       <c r="O36" t="n">
-        <v>0</v>
+        <v>0.0262</v>
       </c>
       <c r="P36" t="n">
-        <v>0</v>
+        <v>0.022</v>
       </c>
       <c r="Q36" t="n">
-        <v>0</v>
+        <v>0.0163</v>
       </c>
       <c r="R36" t="n">
-        <v>0</v>
+        <v>0.0146</v>
       </c>
       <c r="S36" t="n">
-        <v>0</v>
+        <v>0.0144</v>
       </c>
       <c r="T36" t="n">
-        <v>0</v>
+        <v>0.0141</v>
       </c>
       <c r="U36" t="n">
-        <v>0</v>
+        <v>0.0137</v>
       </c>
       <c r="V36" t="n">
-        <v>0</v>
+        <v>0.0068</v>
       </c>
     </row>
     <row r="37">
@@ -3124,7 +3124,7 @@
         <v>0</v>
       </c>
       <c r="M39" t="n">
-        <v>0</v>
+        <v>-0.0003</v>
       </c>
       <c r="N39" t="n">
         <v>0</v>
@@ -3192,34 +3192,34 @@
         <v>0</v>
       </c>
       <c r="M40" t="n">
-        <v>0</v>
+        <v>0.0063</v>
       </c>
       <c r="N40" t="n">
-        <v>0</v>
+        <v>-0.0115</v>
       </c>
       <c r="O40" t="n">
-        <v>0</v>
+        <v>-0.0209</v>
       </c>
       <c r="P40" t="n">
-        <v>0</v>
+        <v>-0.0239</v>
       </c>
       <c r="Q40" t="n">
-        <v>0</v>
+        <v>-0.0296</v>
       </c>
       <c r="R40" t="n">
-        <v>0</v>
+        <v>-0.0123</v>
       </c>
       <c r="S40" t="n">
-        <v>0</v>
+        <v>-0.0032</v>
       </c>
       <c r="T40" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="U40" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="V40" t="n">
-        <v>0</v>
+        <v>-0.0027</v>
       </c>
     </row>
     <row r="41">
@@ -3328,34 +3328,34 @@
         <v>0</v>
       </c>
       <c r="M42" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="N42" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="O42" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="P42" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="Q42" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="R42" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="S42" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="T42" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="U42" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="V42" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
     </row>
     <row r="43">
@@ -3464,34 +3464,34 @@
         <v>0</v>
       </c>
       <c r="M44" t="n">
-        <v>0</v>
+        <v>0.0443</v>
       </c>
       <c r="N44" t="n">
-        <v>0</v>
+        <v>0.1365</v>
       </c>
       <c r="O44" t="n">
-        <v>0</v>
+        <v>0.1324</v>
       </c>
       <c r="P44" t="n">
-        <v>0</v>
+        <v>0.1589</v>
       </c>
       <c r="Q44" t="n">
-        <v>0</v>
+        <v>0.1171</v>
       </c>
       <c r="R44" t="n">
-        <v>0</v>
+        <v>0.0157</v>
       </c>
       <c r="S44" t="n">
-        <v>0</v>
+        <v>0.0154</v>
       </c>
       <c r="T44" t="n">
-        <v>0</v>
+        <v>0.0039</v>
       </c>
       <c r="U44" t="n">
-        <v>0</v>
+        <v>0.0295</v>
       </c>
       <c r="V44" t="n">
-        <v>0</v>
+        <v>-0.1477</v>
       </c>
     </row>
     <row r="45">
@@ -3532,34 +3532,34 @@
         <v>0</v>
       </c>
       <c r="M45" t="n">
-        <v>0</v>
+        <v>12.4</v>
       </c>
       <c r="N45" t="n">
-        <v>0</v>
+        <v>12.5418</v>
       </c>
       <c r="O45" t="n">
-        <v>0</v>
+        <v>12.6917</v>
       </c>
       <c r="P45" t="n">
-        <v>0</v>
+        <v>12.8446</v>
       </c>
       <c r="Q45" t="n">
-        <v>0</v>
+        <v>13.0029</v>
       </c>
       <c r="R45" t="n">
-        <v>0</v>
+        <v>13.1643</v>
       </c>
       <c r="S45" t="n">
-        <v>0</v>
+        <v>13.3218</v>
       </c>
       <c r="T45" t="n">
-        <v>0</v>
+        <v>13.477</v>
       </c>
       <c r="U45" t="n">
-        <v>0</v>
+        <v>13.6268</v>
       </c>
       <c r="V45" t="n">
-        <v>0</v>
+        <v>13.7766</v>
       </c>
     </row>
     <row r="46">
@@ -3600,34 +3600,34 @@
         <v>0</v>
       </c>
       <c r="M46" t="n">
-        <v>0</v>
+        <v>0.4433</v>
       </c>
       <c r="N46" t="n">
-        <v>0</v>
+        <v>-0.0007</v>
       </c>
       <c r="O46" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="P46" t="n">
-        <v>0</v>
+        <v>-0.0003</v>
       </c>
       <c r="Q46" t="n">
-        <v>0</v>
+        <v>-0.0003</v>
       </c>
       <c r="R46" t="n">
-        <v>0</v>
+        <v>-0.0003</v>
       </c>
       <c r="S46" t="n">
-        <v>0</v>
+        <v>-0.0004</v>
       </c>
       <c r="T46" t="n">
-        <v>0</v>
+        <v>-0.0005</v>
       </c>
       <c r="U46" t="n">
-        <v>0</v>
+        <v>-0.0005</v>
       </c>
       <c r="V46" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
     </row>
     <row r="47">
@@ -3872,34 +3872,34 @@
         <v>0</v>
       </c>
       <c r="M50" t="n">
-        <v>0</v>
+        <v>-0.3824</v>
       </c>
       <c r="N50" t="n">
-        <v>0</v>
+        <v>0.0535</v>
       </c>
       <c r="O50" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="P50" t="n">
-        <v>0</v>
+        <v>0.0213</v>
       </c>
       <c r="Q50" t="n">
-        <v>0</v>
+        <v>0.0318</v>
       </c>
       <c r="R50" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="S50" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="T50" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="U50" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="V50" t="n">
-        <v>0</v>
+        <v>-0.1618</v>
       </c>
     </row>
     <row r="51">
@@ -3940,34 +3940,34 @@
         <v>0</v>
       </c>
       <c r="M51" t="n">
-        <v>0</v>
+        <v>-0.0091</v>
       </c>
       <c r="N51" t="n">
-        <v>0</v>
+        <v>0.0003</v>
       </c>
       <c r="O51" t="n">
-        <v>0</v>
+        <v>0.0004</v>
       </c>
       <c r="P51" t="n">
-        <v>0</v>
+        <v>0.0004</v>
       </c>
       <c r="Q51" t="n">
-        <v>0</v>
+        <v>0.0004</v>
       </c>
       <c r="R51" t="n">
-        <v>0</v>
+        <v>0.0004</v>
       </c>
       <c r="S51" t="n">
-        <v>0</v>
+        <v>0.0004</v>
       </c>
       <c r="T51" t="n">
-        <v>0</v>
+        <v>0.0004</v>
       </c>
       <c r="U51" t="n">
-        <v>0</v>
+        <v>0.0004</v>
       </c>
       <c r="V51" t="n">
-        <v>0</v>
+        <v>0.0004</v>
       </c>
     </row>
     <row r="52">
@@ -4008,34 +4008,34 @@
         <v>0</v>
       </c>
       <c r="M52" t="n">
-        <v>0</v>
+        <v>0.0405</v>
       </c>
       <c r="N52" t="n">
-        <v>0</v>
+        <v>0.1015</v>
       </c>
       <c r="O52" t="n">
-        <v>0</v>
+        <v>0.1043</v>
       </c>
       <c r="P52" t="n">
-        <v>0</v>
+        <v>0.1076</v>
       </c>
       <c r="Q52" t="n">
-        <v>0</v>
+        <v>0.068</v>
       </c>
       <c r="R52" t="n">
-        <v>0</v>
+        <v>0.0089</v>
       </c>
       <c r="S52" t="n">
-        <v>0</v>
+        <v>0.0055</v>
       </c>
       <c r="T52" t="n">
-        <v>0</v>
+        <v>0.0015</v>
       </c>
       <c r="U52" t="n">
-        <v>0</v>
+        <v>0.0016</v>
       </c>
       <c r="V52" t="n">
-        <v>0</v>
+        <v>0.0017</v>
       </c>
     </row>
     <row r="53">
@@ -4076,34 +4076,34 @@
         <v>0</v>
       </c>
       <c r="M53" t="n">
-        <v>0</v>
+        <v>-0.0594</v>
       </c>
       <c r="N53" t="n">
-        <v>0</v>
+        <v>-0.0462</v>
       </c>
       <c r="O53" t="n">
-        <v>0</v>
+        <v>-0.0109</v>
       </c>
       <c r="P53" t="n">
-        <v>0</v>
+        <v>-0.0151</v>
       </c>
       <c r="Q53" t="n">
-        <v>0</v>
+        <v>-0.0177</v>
       </c>
       <c r="R53" t="n">
-        <v>0</v>
+        <v>-0.0185</v>
       </c>
       <c r="S53" t="n">
-        <v>0</v>
+        <v>-0.0183</v>
       </c>
       <c r="T53" t="n">
-        <v>0</v>
+        <v>-0.0181</v>
       </c>
       <c r="U53" t="n">
-        <v>0</v>
+        <v>0.0091</v>
       </c>
       <c r="V53" t="n">
-        <v>0</v>
+        <v>0.0032</v>
       </c>
     </row>
     <row r="54">
@@ -4144,7 +4144,7 @@
         <v>0</v>
       </c>
       <c r="M54" t="n">
-        <v>0</v>
+        <v>0.0004</v>
       </c>
       <c r="N54" t="n">
         <v>0</v>
@@ -4351,28 +4351,28 @@
         <v>0</v>
       </c>
       <c r="N57" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="O57" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="P57" t="n">
-        <v>0</v>
+        <v>-0.0003</v>
       </c>
       <c r="Q57" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="R57" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="S57" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="T57" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="U57" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="V57" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
fix: pull forward tax sheet entries and re-create FIM 03-2024 results folder
</commit_message>
<xml_diff>
--- a/results/03-2024/comparison-deflators-03-2024.xlsx
+++ b/results/03-2024/comparison-deflators-03-2024.xlsx
@@ -883,31 +883,31 @@
         <v>0.2796</v>
       </c>
       <c r="N6" t="n">
-        <v>0.16</v>
+        <v>0.1591</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.1199</v>
+        <v>-0.1208</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.2378</v>
+        <v>-0.2387</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.2232</v>
+        <v>-0.2241</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.2835</v>
+        <v>-0.2844</v>
       </c>
       <c r="S6" t="n">
-        <v>-0.2191</v>
+        <v>-0.22</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.1703</v>
+        <v>-0.1712</v>
       </c>
       <c r="U6" t="n">
-        <v>-0.035</v>
+        <v>-0.0359</v>
       </c>
       <c r="V6" t="n">
-        <v>-0.7412</v>
+        <v>-0.7421</v>
       </c>
     </row>
     <row r="7">
@@ -1563,31 +1563,31 @@
         <v>0.2312</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.2678</v>
+        <v>-0.2729</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.6669</v>
+        <v>-0.6719</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.4807</v>
+        <v>-0.4857</v>
       </c>
       <c r="Q16" t="n">
-        <v>-0.2571</v>
+        <v>-0.262</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.8043</v>
+        <v>-0.8091</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.8209</v>
+        <v>-0.8256</v>
       </c>
       <c r="T16" t="n">
-        <v>-0.5283</v>
+        <v>-0.533</v>
       </c>
       <c r="U16" t="n">
-        <v>-0.3389</v>
+        <v>-0.3436</v>
       </c>
       <c r="V16" t="n">
-        <v>-50.7598</v>
+        <v>-50.7644</v>
       </c>
     </row>
     <row r="17">
@@ -2039,31 +2039,31 @@
         <v>-0.027</v>
       </c>
       <c r="N23" t="n">
-        <v>-0.016</v>
+        <v>-0.0202</v>
       </c>
       <c r="O23" t="n">
-        <v>-0.0121</v>
+        <v>-0.0162</v>
       </c>
       <c r="P23" t="n">
-        <v>-0.0046</v>
+        <v>-0.0086</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.0121</v>
+        <v>0.0081</v>
       </c>
       <c r="R23" t="n">
-        <v>0.0263</v>
+        <v>0.0223</v>
       </c>
       <c r="S23" t="n">
-        <v>0.0059</v>
+        <v>0.002</v>
       </c>
       <c r="T23" t="n">
-        <v>0.006</v>
+        <v>0.0021</v>
       </c>
       <c r="U23" t="n">
-        <v>0.011</v>
+        <v>0.0072</v>
       </c>
       <c r="V23" t="n">
-        <v>0.0157</v>
+        <v>0.012</v>
       </c>
     </row>
     <row r="24">
@@ -2512,16 +2512,16 @@
         <v>0</v>
       </c>
       <c r="M30" t="n">
-        <v>-0.0001</v>
+        <v>0</v>
       </c>
       <c r="N30" t="n">
-        <v>0.0028</v>
+        <v>0</v>
       </c>
       <c r="O30" t="n">
-        <v>0.0015</v>
+        <v>0</v>
       </c>
       <c r="P30" t="n">
-        <v>0.0005</v>
+        <v>0</v>
       </c>
       <c r="Q30" t="n">
         <v>0</v>
@@ -2716,34 +2716,34 @@
         <v>0</v>
       </c>
       <c r="M33" t="n">
-        <v>0.4485</v>
+        <v>0</v>
       </c>
       <c r="N33" t="n">
-        <v>-0.0006</v>
+        <v>0</v>
       </c>
       <c r="O33" t="n">
-        <v>0.0003</v>
+        <v>0</v>
       </c>
       <c r="P33" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="Q33" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="R33" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="S33" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="T33" t="n">
-        <v>-0.0004</v>
+        <v>0</v>
       </c>
       <c r="U33" t="n">
-        <v>-0.0004</v>
+        <v>0</v>
       </c>
       <c r="V33" t="n">
-        <v>0.0003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -2784,34 +2784,34 @@
         <v>0</v>
       </c>
       <c r="M34" t="n">
-        <v>-0.0008</v>
+        <v>0</v>
       </c>
       <c r="N34" t="n">
-        <v>-0.0038</v>
+        <v>-0.0009</v>
       </c>
       <c r="O34" t="n">
-        <v>-0.0017</v>
+        <v>-0.0009</v>
       </c>
       <c r="P34" t="n">
-        <v>0.0002</v>
+        <v>-0.0009</v>
       </c>
       <c r="Q34" t="n">
-        <v>0.0011</v>
+        <v>-0.0009</v>
       </c>
       <c r="R34" t="n">
-        <v>0.0011</v>
+        <v>-0.0009</v>
       </c>
       <c r="S34" t="n">
-        <v>0.001</v>
+        <v>-0.0009</v>
       </c>
       <c r="T34" t="n">
-        <v>0.001</v>
+        <v>-0.0009</v>
       </c>
       <c r="U34" t="n">
-        <v>0.0009</v>
+        <v>-0.0009</v>
       </c>
       <c r="V34" t="n">
-        <v>0.0012</v>
+        <v>-0.0009</v>
       </c>
     </row>
     <row r="35">
@@ -2852,34 +2852,34 @@
         <v>0</v>
       </c>
       <c r="M35" t="n">
-        <v>0.0003</v>
+        <v>0</v>
       </c>
       <c r="N35" t="n">
-        <v>0.0296</v>
+        <v>0</v>
       </c>
       <c r="O35" t="n">
-        <v>0.0378</v>
+        <v>0</v>
       </c>
       <c r="P35" t="n">
-        <v>0.0497</v>
+        <v>0</v>
       </c>
       <c r="Q35" t="n">
-        <v>0.0503</v>
+        <v>0</v>
       </c>
       <c r="R35" t="n">
-        <v>0.0233</v>
+        <v>0</v>
       </c>
       <c r="S35" t="n">
-        <v>0.0163</v>
+        <v>0</v>
       </c>
       <c r="T35" t="n">
-        <v>0.0056</v>
+        <v>0</v>
       </c>
       <c r="U35" t="n">
-        <v>0.0045</v>
+        <v>0</v>
       </c>
       <c r="V35" t="n">
-        <v>0.0034</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -2920,34 +2920,34 @@
         <v>0</v>
       </c>
       <c r="M36" t="n">
-        <v>0.0004</v>
+        <v>0</v>
       </c>
       <c r="N36" t="n">
-        <v>0.0155</v>
+        <v>0</v>
       </c>
       <c r="O36" t="n">
-        <v>0.0262</v>
+        <v>0</v>
       </c>
       <c r="P36" t="n">
-        <v>0.022</v>
+        <v>0</v>
       </c>
       <c r="Q36" t="n">
-        <v>0.0163</v>
+        <v>0</v>
       </c>
       <c r="R36" t="n">
-        <v>0.0146</v>
+        <v>0</v>
       </c>
       <c r="S36" t="n">
-        <v>0.0144</v>
+        <v>0</v>
       </c>
       <c r="T36" t="n">
-        <v>0.0141</v>
+        <v>0</v>
       </c>
       <c r="U36" t="n">
-        <v>0.0137</v>
+        <v>0</v>
       </c>
       <c r="V36" t="n">
-        <v>0.0068</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -3124,7 +3124,7 @@
         <v>0</v>
       </c>
       <c r="M39" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="N39" t="n">
         <v>0</v>
@@ -3192,34 +3192,34 @@
         <v>0</v>
       </c>
       <c r="M40" t="n">
-        <v>0.0063</v>
+        <v>0</v>
       </c>
       <c r="N40" t="n">
-        <v>-0.0115</v>
+        <v>0</v>
       </c>
       <c r="O40" t="n">
-        <v>-0.0209</v>
+        <v>0</v>
       </c>
       <c r="P40" t="n">
-        <v>-0.0239</v>
+        <v>0</v>
       </c>
       <c r="Q40" t="n">
-        <v>-0.0296</v>
+        <v>0</v>
       </c>
       <c r="R40" t="n">
-        <v>-0.0123</v>
+        <v>0</v>
       </c>
       <c r="S40" t="n">
-        <v>-0.0032</v>
+        <v>0</v>
       </c>
       <c r="T40" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c r="U40" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c r="V40" t="n">
-        <v>-0.0027</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -3328,34 +3328,34 @@
         <v>0</v>
       </c>
       <c r="M42" t="n">
-        <v>-0.0001</v>
+        <v>0</v>
       </c>
       <c r="N42" t="n">
-        <v>-0.0001</v>
+        <v>0</v>
       </c>
       <c r="O42" t="n">
-        <v>-0.0001</v>
+        <v>0</v>
       </c>
       <c r="P42" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c r="Q42" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c r="R42" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c r="S42" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c r="T42" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c r="U42" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c r="V42" t="n">
-        <v>-0.0001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -3464,34 +3464,34 @@
         <v>0</v>
       </c>
       <c r="M44" t="n">
-        <v>0.0443</v>
+        <v>0</v>
       </c>
       <c r="N44" t="n">
-        <v>0.1365</v>
+        <v>-0.0051</v>
       </c>
       <c r="O44" t="n">
-        <v>0.1324</v>
+        <v>-0.005</v>
       </c>
       <c r="P44" t="n">
-        <v>0.1589</v>
+        <v>-0.0049</v>
       </c>
       <c r="Q44" t="n">
-        <v>0.1171</v>
+        <v>-0.0049</v>
       </c>
       <c r="R44" t="n">
-        <v>0.0157</v>
+        <v>-0.0048</v>
       </c>
       <c r="S44" t="n">
-        <v>0.0154</v>
+        <v>-0.0047</v>
       </c>
       <c r="T44" t="n">
-        <v>0.0039</v>
+        <v>-0.0047</v>
       </c>
       <c r="U44" t="n">
-        <v>0.0295</v>
+        <v>-0.0046</v>
       </c>
       <c r="V44" t="n">
-        <v>-0.1477</v>
+        <v>-0.0046</v>
       </c>
     </row>
     <row r="45">
@@ -3532,34 +3532,34 @@
         <v>0</v>
       </c>
       <c r="M45" t="n">
-        <v>12.4</v>
+        <v>0</v>
       </c>
       <c r="N45" t="n">
-        <v>12.5418</v>
+        <v>0</v>
       </c>
       <c r="O45" t="n">
-        <v>12.6917</v>
+        <v>0</v>
       </c>
       <c r="P45" t="n">
-        <v>12.8446</v>
+        <v>0</v>
       </c>
       <c r="Q45" t="n">
-        <v>13.0029</v>
+        <v>0</v>
       </c>
       <c r="R45" t="n">
-        <v>13.1643</v>
+        <v>0</v>
       </c>
       <c r="S45" t="n">
-        <v>13.3218</v>
+        <v>0</v>
       </c>
       <c r="T45" t="n">
-        <v>13.477</v>
+        <v>0</v>
       </c>
       <c r="U45" t="n">
-        <v>13.6268</v>
+        <v>0</v>
       </c>
       <c r="V45" t="n">
-        <v>13.7766</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -3600,34 +3600,34 @@
         <v>0</v>
       </c>
       <c r="M46" t="n">
-        <v>0.4433</v>
+        <v>0</v>
       </c>
       <c r="N46" t="n">
-        <v>-0.0007</v>
+        <v>0</v>
       </c>
       <c r="O46" t="n">
-        <v>0.0002</v>
+        <v>0</v>
       </c>
       <c r="P46" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="Q46" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="R46" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="S46" t="n">
-        <v>-0.0004</v>
+        <v>0</v>
       </c>
       <c r="T46" t="n">
-        <v>-0.0005</v>
+        <v>0</v>
       </c>
       <c r="U46" t="n">
-        <v>-0.0005</v>
+        <v>0</v>
       </c>
       <c r="V46" t="n">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -3872,34 +3872,34 @@
         <v>0</v>
       </c>
       <c r="M50" t="n">
-        <v>-0.3824</v>
+        <v>0</v>
       </c>
       <c r="N50" t="n">
-        <v>0.0535</v>
+        <v>0</v>
       </c>
       <c r="O50" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c r="P50" t="n">
-        <v>0.0213</v>
+        <v>0</v>
       </c>
       <c r="Q50" t="n">
-        <v>0.0318</v>
+        <v>0</v>
       </c>
       <c r="R50" t="n">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="S50" t="n">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="T50" t="n">
-        <v>0.0002</v>
+        <v>0</v>
       </c>
       <c r="U50" t="n">
-        <v>0.0002</v>
+        <v>0</v>
       </c>
       <c r="V50" t="n">
-        <v>-0.1618</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -3940,34 +3940,34 @@
         <v>0</v>
       </c>
       <c r="M51" t="n">
-        <v>-0.0091</v>
+        <v>0</v>
       </c>
       <c r="N51" t="n">
-        <v>0.0003</v>
+        <v>-0.0042</v>
       </c>
       <c r="O51" t="n">
-        <v>0.0004</v>
+        <v>-0.0041</v>
       </c>
       <c r="P51" t="n">
-        <v>0.0004</v>
+        <v>-0.0041</v>
       </c>
       <c r="Q51" t="n">
-        <v>0.0004</v>
+        <v>-0.004</v>
       </c>
       <c r="R51" t="n">
-        <v>0.0004</v>
+        <v>-0.0039</v>
       </c>
       <c r="S51" t="n">
-        <v>0.0004</v>
+        <v>-0.0039</v>
       </c>
       <c r="T51" t="n">
-        <v>0.0004</v>
+        <v>-0.0038</v>
       </c>
       <c r="U51" t="n">
-        <v>0.0004</v>
+        <v>-0.0038</v>
       </c>
       <c r="V51" t="n">
-        <v>0.0004</v>
+        <v>-0.0037</v>
       </c>
     </row>
     <row r="52">
@@ -4008,34 +4008,34 @@
         <v>0</v>
       </c>
       <c r="M52" t="n">
-        <v>0.0405</v>
+        <v>0</v>
       </c>
       <c r="N52" t="n">
-        <v>0.1015</v>
+        <v>0</v>
       </c>
       <c r="O52" t="n">
-        <v>0.1043</v>
+        <v>0</v>
       </c>
       <c r="P52" t="n">
-        <v>0.1076</v>
+        <v>0</v>
       </c>
       <c r="Q52" t="n">
-        <v>0.068</v>
+        <v>0</v>
       </c>
       <c r="R52" t="n">
-        <v>0.0089</v>
+        <v>0</v>
       </c>
       <c r="S52" t="n">
-        <v>0.0055</v>
+        <v>0</v>
       </c>
       <c r="T52" t="n">
-        <v>0.0015</v>
+        <v>0</v>
       </c>
       <c r="U52" t="n">
-        <v>0.0016</v>
+        <v>0</v>
       </c>
       <c r="V52" t="n">
-        <v>0.0017</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -4076,34 +4076,34 @@
         <v>0</v>
       </c>
       <c r="M53" t="n">
-        <v>-0.0594</v>
+        <v>0</v>
       </c>
       <c r="N53" t="n">
-        <v>-0.0462</v>
+        <v>0</v>
       </c>
       <c r="O53" t="n">
-        <v>-0.0109</v>
+        <v>0</v>
       </c>
       <c r="P53" t="n">
-        <v>-0.0151</v>
+        <v>0</v>
       </c>
       <c r="Q53" t="n">
-        <v>-0.0177</v>
+        <v>0</v>
       </c>
       <c r="R53" t="n">
-        <v>-0.0185</v>
+        <v>0</v>
       </c>
       <c r="S53" t="n">
-        <v>-0.0183</v>
+        <v>0</v>
       </c>
       <c r="T53" t="n">
-        <v>-0.0181</v>
+        <v>0</v>
       </c>
       <c r="U53" t="n">
-        <v>0.0091</v>
+        <v>0</v>
       </c>
       <c r="V53" t="n">
-        <v>0.0032</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -4144,7 +4144,7 @@
         <v>0</v>
       </c>
       <c r="M54" t="n">
-        <v>0.0004</v>
+        <v>0</v>
       </c>
       <c r="N54" t="n">
         <v>0</v>
@@ -4351,28 +4351,28 @@
         <v>0</v>
       </c>
       <c r="N57" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c r="O57" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c r="P57" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="Q57" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c r="R57" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c r="S57" t="n">
-        <v>-0.0001</v>
+        <v>0</v>
       </c>
       <c r="T57" t="n">
-        <v>-0.0001</v>
+        <v>0</v>
       </c>
       <c r="U57" t="n">
-        <v>-0.0001</v>
+        <v>0</v>
       </c>
       <c r="V57" t="n">
         <v>0</v>
@@ -4416,16 +4416,16 @@
         <v>0.0064</v>
       </c>
       <c r="M58" t="n">
-        <v>0.0045</v>
+        <v>0.0044</v>
       </c>
       <c r="N58" t="n">
-        <v>0.0046</v>
+        <v>0.0074</v>
       </c>
       <c r="O58" t="n">
-        <v>0.0053</v>
+        <v>0.0067</v>
       </c>
       <c r="P58" t="n">
-        <v>0.0055</v>
+        <v>0.006</v>
       </c>
       <c r="Q58" t="n">
         <v>0.0055</v>
@@ -4567,7 +4567,7 @@
         <v>-0.029</v>
       </c>
       <c r="R60" t="n">
-        <v>-0.0281</v>
+        <v>-0.028</v>
       </c>
       <c r="S60" t="n">
         <v>-0.0264</v>
@@ -4620,34 +4620,34 @@
         <v>-0.0421</v>
       </c>
       <c r="M61" t="n">
-        <v>-0.2947</v>
+        <v>0.1538</v>
       </c>
       <c r="N61" t="n">
-        <v>-0.2553</v>
+        <v>-0.2559</v>
       </c>
       <c r="O61" t="n">
-        <v>-0.4625</v>
+        <v>-0.4623</v>
       </c>
       <c r="P61" t="n">
-        <v>-0.0666</v>
+        <v>-0.0669</v>
       </c>
       <c r="Q61" t="n">
-        <v>-0.083</v>
+        <v>-0.0832</v>
       </c>
       <c r="R61" t="n">
-        <v>-0.4212</v>
+        <v>-0.4215</v>
       </c>
       <c r="S61" t="n">
-        <v>-0.2973</v>
+        <v>-0.2976</v>
       </c>
       <c r="T61" t="n">
-        <v>-0.1303</v>
+        <v>-0.1307</v>
       </c>
       <c r="U61" t="n">
-        <v>-0.166</v>
+        <v>-0.1664</v>
       </c>
       <c r="V61" t="n">
-        <v>-1.9434</v>
+        <v>-1.9431</v>
       </c>
     </row>
     <row r="62">
@@ -4688,34 +4688,34 @@
         <v>0.3088</v>
       </c>
       <c r="M62" t="n">
-        <v>0.2804</v>
+        <v>0.2796</v>
       </c>
       <c r="N62" t="n">
-        <v>0.1638</v>
+        <v>0.16</v>
       </c>
       <c r="O62" t="n">
-        <v>-0.1183</v>
+        <v>-0.1199</v>
       </c>
       <c r="P62" t="n">
-        <v>-0.2381</v>
+        <v>-0.2378</v>
       </c>
       <c r="Q62" t="n">
-        <v>-0.2242</v>
+        <v>-0.2232</v>
       </c>
       <c r="R62" t="n">
-        <v>-0.2846</v>
+        <v>-0.2835</v>
       </c>
       <c r="S62" t="n">
-        <v>-0.2202</v>
+        <v>-0.2191</v>
       </c>
       <c r="T62" t="n">
-        <v>-0.1713</v>
+        <v>-0.1703</v>
       </c>
       <c r="U62" t="n">
-        <v>-0.0359</v>
+        <v>-0.035</v>
       </c>
       <c r="V62" t="n">
-        <v>-0.7425</v>
+        <v>-0.7412</v>
       </c>
     </row>
     <row r="63">
@@ -4756,34 +4756,34 @@
         <v>-0.2751</v>
       </c>
       <c r="M63" t="n">
-        <v>-0.1625</v>
+        <v>-0.1622</v>
       </c>
       <c r="N63" t="n">
-        <v>-0.2623</v>
+        <v>-0.2326</v>
       </c>
       <c r="O63" t="n">
-        <v>-0.2571</v>
+        <v>-0.2193</v>
       </c>
       <c r="P63" t="n">
-        <v>-0.0697</v>
+        <v>-0.0199</v>
       </c>
       <c r="Q63" t="n">
-        <v>-0.1072</v>
+        <v>-0.0569</v>
       </c>
       <c r="R63" t="n">
-        <v>-0.0109</v>
+        <v>0.0123</v>
       </c>
       <c r="S63" t="n">
-        <v>0.0136</v>
+        <v>0.0299</v>
       </c>
       <c r="T63" t="n">
-        <v>0.0369</v>
+        <v>0.0425</v>
       </c>
       <c r="U63" t="n">
-        <v>0.0515</v>
+        <v>0.056</v>
       </c>
       <c r="V63" t="n">
-        <v>0.0668</v>
+        <v>0.0702</v>
       </c>
     </row>
     <row r="64">
@@ -4824,34 +4824,34 @@
         <v>0.3669</v>
       </c>
       <c r="M64" t="n">
-        <v>0.3655</v>
+        <v>0.3659</v>
       </c>
       <c r="N64" t="n">
-        <v>0.2297</v>
+        <v>0.2453</v>
       </c>
       <c r="O64" t="n">
-        <v>0.1811</v>
+        <v>0.2073</v>
       </c>
       <c r="P64" t="n">
-        <v>0.3253</v>
+        <v>0.3473</v>
       </c>
       <c r="Q64" t="n">
-        <v>0.2391</v>
+        <v>0.2554</v>
       </c>
       <c r="R64" t="n">
-        <v>-0.1013</v>
+        <v>-0.0867</v>
       </c>
       <c r="S64" t="n">
-        <v>-0.1198</v>
+        <v>-0.1053</v>
       </c>
       <c r="T64" t="n">
-        <v>-0.0931</v>
+        <v>-0.079</v>
       </c>
       <c r="U64" t="n">
-        <v>-0.0867</v>
+        <v>-0.073</v>
       </c>
       <c r="V64" t="n">
-        <v>-0.0102</v>
+        <v>-0.0034</v>
       </c>
     </row>
     <row r="65">
@@ -4969,13 +4969,13 @@
         <v>-0.0488</v>
       </c>
       <c r="P66" t="n">
-        <v>-0.0432</v>
+        <v>-0.0433</v>
       </c>
       <c r="Q66" t="n">
         <v>-0.0257</v>
       </c>
       <c r="R66" t="n">
-        <v>-0.0102</v>
+        <v>-0.0103</v>
       </c>
       <c r="S66" t="n">
         <v>-0.0098</v>
@@ -5028,7 +5028,7 @@
         <v>0.0098</v>
       </c>
       <c r="M67" t="n">
-        <v>0.01</v>
+        <v>0.0098</v>
       </c>
       <c r="N67" t="n">
         <v>0.0059</v>
@@ -5096,34 +5096,34 @@
         <v>0.0114</v>
       </c>
       <c r="M68" t="n">
-        <v>-0.1543</v>
+        <v>-0.1481</v>
       </c>
       <c r="N68" t="n">
-        <v>-0.1614</v>
+        <v>-0.173</v>
       </c>
       <c r="O68" t="n">
-        <v>-0.0594</v>
+        <v>-0.0803</v>
       </c>
       <c r="P68" t="n">
-        <v>-0.0121</v>
+        <v>-0.036</v>
       </c>
       <c r="Q68" t="n">
-        <v>-0.0002</v>
+        <v>-0.0298</v>
       </c>
       <c r="R68" t="n">
-        <v>-0.044</v>
+        <v>-0.0563</v>
       </c>
       <c r="S68" t="n">
-        <v>-0.0481</v>
+        <v>-0.0513</v>
       </c>
       <c r="T68" t="n">
-        <v>-0.0504</v>
+        <v>-0.0506</v>
       </c>
       <c r="U68" t="n">
-        <v>-0.1048</v>
+        <v>-0.105</v>
       </c>
       <c r="V68" t="n">
-        <v>-6.302</v>
+        <v>-6.3047</v>
       </c>
     </row>
     <row r="69">
@@ -5232,34 +5232,34 @@
         <v>-0.3432</v>
       </c>
       <c r="M70" t="n">
-        <v>-0.1407</v>
+        <v>-0.1408</v>
       </c>
       <c r="N70" t="n">
-        <v>-0.1034</v>
+        <v>-0.1035</v>
       </c>
       <c r="O70" t="n">
-        <v>-0.2904</v>
+        <v>-0.2906</v>
       </c>
       <c r="P70" t="n">
-        <v>-0.2614</v>
+        <v>-0.2615</v>
       </c>
       <c r="Q70" t="n">
-        <v>-0.1046</v>
+        <v>-0.1048</v>
       </c>
       <c r="R70" t="n">
-        <v>-0.0568</v>
+        <v>-0.057</v>
       </c>
       <c r="S70" t="n">
-        <v>-0.0915</v>
+        <v>-0.0917</v>
       </c>
       <c r="T70" t="n">
-        <v>-0.0676</v>
+        <v>-0.0677</v>
       </c>
       <c r="U70" t="n">
-        <v>-0.0296</v>
+        <v>-0.0298</v>
       </c>
       <c r="V70" t="n">
-        <v>-0.0777</v>
+        <v>-0.0778</v>
       </c>
     </row>
     <row r="71">
@@ -5368,34 +5368,34 @@
         <v>0.5287</v>
       </c>
       <c r="M72" t="n">
-        <v>0.1869</v>
+        <v>0.2312</v>
       </c>
       <c r="N72" t="n">
-        <v>-0.4043</v>
+        <v>-0.2678</v>
       </c>
       <c r="O72" t="n">
-        <v>-0.7993</v>
+        <v>-0.6669</v>
       </c>
       <c r="P72" t="n">
-        <v>-0.6397</v>
+        <v>-0.4807</v>
       </c>
       <c r="Q72" t="n">
-        <v>-0.3742</v>
+        <v>-0.2571</v>
       </c>
       <c r="R72" t="n">
-        <v>-0.82</v>
+        <v>-0.8043</v>
       </c>
       <c r="S72" t="n">
-        <v>-0.8363</v>
+        <v>-0.8209</v>
       </c>
       <c r="T72" t="n">
-        <v>-0.5322</v>
+        <v>-0.5283</v>
       </c>
       <c r="U72" t="n">
-        <v>-0.3685</v>
+        <v>-0.3389</v>
       </c>
       <c r="V72" t="n">
-        <v>-50.6121</v>
+        <v>-50.7598</v>
       </c>
     </row>
     <row r="73">
@@ -5436,34 +5436,34 @@
         <v>27610.1</v>
       </c>
       <c r="M73" t="n">
-        <v>27944.6</v>
+        <v>27957</v>
       </c>
       <c r="N73" t="n">
-        <v>28264.1826</v>
+        <v>28276.7244</v>
       </c>
       <c r="O73" t="n">
-        <v>28601.9138</v>
+        <v>28614.6055</v>
       </c>
       <c r="P73" t="n">
-        <v>28946.529</v>
+        <v>28959.3736</v>
       </c>
       <c r="Q73" t="n">
-        <v>29303.3476</v>
+        <v>29316.3505</v>
       </c>
       <c r="R73" t="n">
-        <v>29666.9459</v>
+        <v>29680.1101</v>
       </c>
       <c r="S73" t="n">
-        <v>30021.887</v>
+        <v>30035.2088</v>
       </c>
       <c r="T73" t="n">
-        <v>30371.8216</v>
+        <v>30385.2987</v>
       </c>
       <c r="U73" t="n">
-        <v>30709.2399</v>
+        <v>30722.8667</v>
       </c>
       <c r="V73" t="n">
-        <v>31046.8669</v>
+        <v>31060.6435</v>
       </c>
     </row>
     <row r="74">
@@ -5504,34 +5504,34 @@
         <v>-0.3502</v>
       </c>
       <c r="M74" t="n">
-        <v>-0.2978</v>
+        <v>0.1455</v>
       </c>
       <c r="N74" t="n">
-        <v>-0.1183</v>
+        <v>-0.119</v>
       </c>
       <c r="O74" t="n">
-        <v>-0.3518</v>
+        <v>-0.3516</v>
       </c>
       <c r="P74" t="n">
-        <v>-0.0102</v>
+        <v>-0.0106</v>
       </c>
       <c r="Q74" t="n">
-        <v>0.0156</v>
+        <v>0.0153</v>
       </c>
       <c r="R74" t="n">
-        <v>-0.3044</v>
+        <v>-0.3047</v>
       </c>
       <c r="S74" t="n">
-        <v>-0.1891</v>
+        <v>-0.1895</v>
       </c>
       <c r="T74" t="n">
-        <v>-0.0358</v>
+        <v>-0.0363</v>
       </c>
       <c r="U74" t="n">
-        <v>-0.0869</v>
+        <v>-0.0874</v>
       </c>
       <c r="V74" t="n">
-        <v>-1.6968</v>
+        <v>-1.6966</v>
       </c>
     </row>
     <row r="75">
@@ -5649,16 +5649,16 @@
         <v>-0.1051</v>
       </c>
       <c r="P76" t="n">
-        <v>-0.102</v>
+        <v>-0.1019</v>
       </c>
       <c r="Q76" t="n">
-        <v>-0.0999</v>
+        <v>-0.0998</v>
       </c>
       <c r="R76" t="n">
-        <v>-0.0968</v>
+        <v>-0.0967</v>
       </c>
       <c r="S76" t="n">
-        <v>-0.0938</v>
+        <v>-0.0937</v>
       </c>
       <c r="T76" t="n">
         <v>-0.001</v>
@@ -5776,34 +5776,34 @@
         <v>0.6465</v>
       </c>
       <c r="M78" t="n">
-        <v>0.6308</v>
+        <v>0.2484</v>
       </c>
       <c r="N78" t="n">
-        <v>0.0461</v>
+        <v>0.0996</v>
       </c>
       <c r="O78" t="n">
-        <v>0.3614</v>
+        <v>0.3612</v>
       </c>
       <c r="P78" t="n">
-        <v>-0.065</v>
+        <v>-0.0437</v>
       </c>
       <c r="Q78" t="n">
-        <v>-0.0943</v>
+        <v>-0.0625</v>
       </c>
       <c r="R78" t="n">
-        <v>0.2326</v>
+        <v>0.2327</v>
       </c>
       <c r="S78" t="n">
-        <v>0.121</v>
+        <v>0.1212</v>
       </c>
       <c r="T78" t="n">
-        <v>-0.0294</v>
+        <v>-0.0292</v>
       </c>
       <c r="U78" t="n">
-        <v>0.0159</v>
+        <v>0.0161</v>
       </c>
       <c r="V78" t="n">
-        <v>-41.5341</v>
+        <v>-41.6959</v>
       </c>
     </row>
     <row r="79">
@@ -5844,34 +5844,34 @@
         <v>-0.0209</v>
       </c>
       <c r="M79" t="n">
-        <v>-0.018</v>
+        <v>-0.027</v>
       </c>
       <c r="N79" t="n">
-        <v>-0.0163</v>
+        <v>-0.016</v>
       </c>
       <c r="O79" t="n">
-        <v>-0.0125</v>
+        <v>-0.0121</v>
       </c>
       <c r="P79" t="n">
-        <v>-0.005</v>
+        <v>-0.0046</v>
       </c>
       <c r="Q79" t="n">
-        <v>0.0117</v>
+        <v>0.0121</v>
       </c>
       <c r="R79" t="n">
-        <v>0.0258</v>
+        <v>0.0263</v>
       </c>
       <c r="S79" t="n">
-        <v>0.0055</v>
+        <v>0.0059</v>
       </c>
       <c r="T79" t="n">
-        <v>0.0055</v>
+        <v>0.006</v>
       </c>
       <c r="U79" t="n">
-        <v>0.0106</v>
+        <v>0.011</v>
       </c>
       <c r="V79" t="n">
-        <v>0.0154</v>
+        <v>0.0157</v>
       </c>
     </row>
     <row r="80">
@@ -5912,34 +5912,34 @@
         <v>0.219</v>
       </c>
       <c r="M80" t="n">
-        <v>0.017</v>
+        <v>0.0574</v>
       </c>
       <c r="N80" t="n">
-        <v>0.0491</v>
+        <v>0.1506</v>
       </c>
       <c r="O80" t="n">
-        <v>-0.0678</v>
+        <v>0.0366</v>
       </c>
       <c r="P80" t="n">
-        <v>-0.1386</v>
+        <v>-0.0311</v>
       </c>
       <c r="Q80" t="n">
-        <v>0.0267</v>
+        <v>0.0947</v>
       </c>
       <c r="R80" t="n">
-        <v>-0.0564</v>
+        <v>-0.0475</v>
       </c>
       <c r="S80" t="n">
-        <v>-0.0342</v>
+        <v>-0.0287</v>
       </c>
       <c r="T80" t="n">
-        <v>-0.0129</v>
+        <v>-0.0114</v>
       </c>
       <c r="U80" t="n">
-        <v>-0.0064</v>
+        <v>-0.0048</v>
       </c>
       <c r="V80" t="n">
-        <v>0.0002</v>
+        <v>0.0019</v>
       </c>
     </row>
     <row r="81">
@@ -5980,34 +5980,34 @@
         <v>0.1954</v>
       </c>
       <c r="M81" t="n">
-        <v>0.1982</v>
+        <v>0.1388</v>
       </c>
       <c r="N81" t="n">
-        <v>0.2155</v>
+        <v>0.1693</v>
       </c>
       <c r="O81" t="n">
-        <v>0.1739</v>
+        <v>0.163</v>
       </c>
       <c r="P81" t="n">
-        <v>0.1286</v>
+        <v>0.1135</v>
       </c>
       <c r="Q81" t="n">
-        <v>0.0951</v>
+        <v>0.0774</v>
       </c>
       <c r="R81" t="n">
-        <v>0.0543</v>
+        <v>0.0358</v>
       </c>
       <c r="S81" t="n">
-        <v>-0.0199</v>
+        <v>-0.0382</v>
       </c>
       <c r="T81" t="n">
-        <v>0.0079</v>
+        <v>-0.0102</v>
       </c>
       <c r="U81" t="n">
-        <v>-0.0105</v>
+        <v>-0.0014</v>
       </c>
       <c r="V81" t="n">
-        <v>-0.0056</v>
+        <v>-0.0023</v>
       </c>
     </row>
     <row r="82">
@@ -6048,7 +6048,7 @@
         <v>0.0141</v>
       </c>
       <c r="M82" t="n">
-        <v>0.0012</v>
+        <v>0.0016</v>
       </c>
       <c r="N82" t="n">
         <v>0.0074</v>
@@ -6255,25 +6255,25 @@
         <v>-0.0005</v>
       </c>
       <c r="N85" t="n">
-        <v>-0.0011</v>
+        <v>-0.0013</v>
       </c>
       <c r="O85" t="n">
-        <v>0.0046</v>
+        <v>0.0043</v>
       </c>
       <c r="P85" t="n">
-        <v>0.0064</v>
+        <v>0.0061</v>
       </c>
       <c r="Q85" t="n">
-        <v>0.006</v>
+        <v>0.0057</v>
       </c>
       <c r="R85" t="n">
+        <v>0.0059</v>
+      </c>
+      <c r="S85" t="n">
         <v>0.0061</v>
       </c>
-      <c r="S85" t="n">
-        <v>0.0062</v>
-      </c>
       <c r="T85" t="n">
-        <v>0.005</v>
+        <v>0.0049</v>
       </c>
       <c r="U85" t="n">
         <v>0.0024</v>

</xml_diff>